<commit_message>
chore: sync go-live updates, manuals, and chatGPT handoff docs
</commit_message>
<xml_diff>
--- a/menual/에이아이챗봇_통합_사용자_참조시트_20260221.xlsx
+++ b/menual/에이아이챗봇_통합_사용자_참조시트_20260221.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -497,7 +497,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>S1(하드닝), S2(종합보고서), S3(UTF-8 검증)</t>
+          <t>S1(20260221 하드닝), S2(202603XX 종합보고서), S3(Go-Live Gap Closure), S4(spec_sync_report), S5(golive 증적)</t>
         </is>
       </c>
     </row>
@@ -522,6 +522,18 @@
       <c r="B5" s="2" t="inlineStr">
         <is>
           <t>운영 지표는 UTC 기준</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>최신 반영 범위</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Node 22 표준화, role/access_level 정규화, MFA/세션, RBAC 2인 승인, audit chain verify, runbook 3종</t>
         </is>
       </c>
     </row>
@@ -536,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -586,192 +598,320 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>M-001</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>stale permission은 401</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>docs\review\plans\20260221_auth_rbac_ops_admin_design_and_hardening_plan.md</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>docs/review/plans/20260221_auth_rbac_ops_admin_design_and_hardening_plan.md</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>AUTH_STALE_PERMISSION</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>2026-02-21T09:32:47Z</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>M-002</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>lockout은 429</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>docs\review\plans\20260221_auth_rbac_ops_admin_design_and_hardening_plan.md</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>docs/review/plans/20260221_auth_rbac_ops_admin_design_and_hardening_plan.md</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>AUTH_LOCKED</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>2026-02-21T09:32:47Z</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>M-003</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>refresh reuse는 409</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>docs\review\plans\20260221_auth_rbac_ops_admin_design_and_hardening_plan.md</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>docs/review/plans/20260221_auth_rbac_ops_admin_design_and_hardening_plan.md</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>AUTH_REFRESH_REUSE_DETECTED</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>2026-02-21T09:32:47Z</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>M-004</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>UTC 지표 집계</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>docs\review\plans\20260221_auth_rbac_ops_admin_design_and_hardening_plan.md</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>UTC</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>2026-02-21T09:32:47Z</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PUBLIC/AUTHENTICATED는 access_level로 분리</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>docs/review/plans/202603XX_go_live_gap_closure_plan.md</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>access_level</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>M-005</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>오류코드 표준 포맷</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>docs\reports\PROJECT_FULL_IMPLEMENTATION_AND_HARDENING_REPORT_20260221.md</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>error_code</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>2026-02-21T09:32:47Z</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>spec_consistency_check FAIL=0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>docs/review/mvp_verification_pack/artifacts/golive_spec_consistency_after.txt</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PASS=9 FAIL=0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>M-006</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>UTF-8 strict decode</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>docs\review\mvp_verification_pack\artifacts\project_full_report_utf8_check_20260221.txt</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>UTF-8 strict decode: PASS</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>2026-02-21T09:32:47Z</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Node 22 표준화(.nvmrc)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>docs/reports/PROJECT_FULL_IMPLEMENTATION_AND_HARDENING_REPORT_202603XX.md</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>.nvmrc=22</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>M-007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Audit Chain Verify API 반영</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>docs/reports/PROJECT_FULL_IMPLEMENTATION_AND_HARDENING_REPORT_202603XX.md</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>/v1/admin/audit-logs/chain-verify</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>M-008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Notion 동기화 완료 상태</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>docs/review/mvp_verification_pack/artifacts/golive_notion_sync_status.txt</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Status: DONE</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>M-009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Go-Live UTF-8 검증 통과</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>docs/review/mvp_verification_pack/artifacts/golive_utf8_check.txt</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>result=PASS</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>M-010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>운영 runbook 3종 반영</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>docs/ops/runbook_scheduler_lock.md</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>runbook</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2026-02-21T12:19:00Z</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -788,7 +928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -847,6 +987,50 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>v2026.02.21-golive</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2026-02-21 21:17:31 +0900</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Go-Live 기준 반영(노드22, access_level 정규화, MFA/세션, RBAC 2인승인, audit chain verify, runbook, Notion 상태)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>S1,S2,S3,S4,S5,S6,S7</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>v2026.02.21-golive</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026-02-21 21:19:00 +0900</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Go-Live 기준 반영(노드22, access_level 정규화, MFA/세션, RBAC 2인승인, audit chain verify, runbook, Notion 상태)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>S1,S2,S3,S4,S5,S6,S7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -858,7 +1042,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1448,6 +1632,216 @@
       <c r="J11" s="2" t="inlineStr">
         <is>
           <t>S1,S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>access_level</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>접근수준 표기</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ROLE이 아닌 공개/인증필요 접근 속성</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ROLE 혼용 방지</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>API 스펙 비고</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>권한 칼럼과 구분해 읽기</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>권한(ROLE)과 혼동 금지</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MFA</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>다중 인증</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>비밀번호 외에 추가 인증(TOTP 등)을 요구하는 보안 방식</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>관리자 계정 탈취 위험 감소</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>OPS/ADMIN 로그인</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>코드 입력/복구코드 보관</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>반복 실패 시 잠금 가능</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_INVALID_CODE/AUTH_MFA_LOCKED</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>audit chain verify</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>감사체인 무결성 점검</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>감사로그 hash chain이 끊기지 않았는지 검증하는 절차/API</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>위변조 조기 탐지</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>운영 점검/감사</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>이상 시 runbook 따라 대응</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>검증 실패 시 export 제한 검토</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>session revoke</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>세션 강제 종료</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>내 세션 목록에서 의심 세션을 종료하거나 타 세션을 일괄 종료</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>계정 도난 대응 속도 향상</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>보안 설정 화면</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>의심 세션 즉시 종료</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>현재 세션과 타 세션 구분</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>runbook</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>운영 대응 절차서</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>장애/보안 이슈 발생 시 단계별 확인·복구 절차를 정리한 문서</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>사고 대응 표준화</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>운영 문서</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>장애시 문서 순서대로 수행</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>임의 조치 금지</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1620,17 +2014,17 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>권한정책 관리</t>
+          <t>RBAC 변경요청 생성/승인</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>OPS 전용 조치</t>
+          <t>OPS 전용 차단조치 직접 실행</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>RBAC Matrix</t>
+          <t>RBAC Matrix/Approval</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -1640,12 +2034,12 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>정책 변경 후 공지</t>
+          <t>직접 적용이 아닌 승인흐름 준수</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>S1,S2</t>
+          <t>S1,S2,S3</t>
         </is>
       </c>
     </row>
@@ -1662,17 +2056,17 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>지표/감사/차단</t>
+          <t>지표/감사/차단/체인검증</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>권한정책 수정</t>
+          <t>RBAC 정책 승인</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>Dashboard/Audit</t>
+          <t>Dashboard/Audit/Chain Verify</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -1682,12 +2076,12 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>차단 사유 기록</t>
+          <t>export 범위 제한 준수</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>S1,S2</t>
+          <t>S1,S2,S3</t>
         </is>
       </c>
     </row>
@@ -1744,7 +2138,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1986,7 +2380,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>권한 변경</t>
+          <t>권한 변경 요청 생성</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -1996,22 +2390,22 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>변경결과</t>
+          <t>변경요청(PENDING)</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>AUTH_STALE_PERMISSION</t>
+          <t>SEC-002-403</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>영향 공지</t>
+          <t>직접 적용이 아닌 승인 대기</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>S1,S2</t>
+          <t>S2,S3</t>
         </is>
       </c>
     </row>
@@ -2052,6 +2446,174 @@
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RBAC 승인요청</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ADMIN(SYSTEM_ADMIN)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>요청 승인/반려</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>request_id/사유</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>APPROVED/REJECTED</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>SEC-002-403</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>요청자 본인승인 금지</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>S2,S3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MFA 설정</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>OPS,ADMIN</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>TOTP 등록/활성화</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>인증앱 코드</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>MFA 활성 상태</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_SETUP_REQUIRED</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>복구코드 안전보관</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>내 세션 관리</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>인증 사용자</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>세션 목록 조회/강제종료</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>세션 선택</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>revoke 결과</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>SEC-001-401</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>의심 세션 즉시 revoke</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audit Chain Verify</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>감사 체인 무결성 점검</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>tenant/기간</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>검증 PASS/FAIL</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>SEC-002-403</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>실패 시 runbook 즉시 실행</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>S2</t>
         </is>
@@ -2068,7 +2630,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2271,6 +2833,117 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>OPS/ADMIN 로그인</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MFA 필요 여부/챌린지 검증</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2차 인증 완료 후 로그인</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>401/429</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_INVALID_CODE/AUTH_MFA_LOCKED</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>RBAC 변경 요청</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>요청 생성 -&gt; 2인 승인</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>승인 후 정책 반영</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>403/409</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>SEC-002-403</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>S2,S3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>감사 무결성 점검</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>chain-verify 실행</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PASS 보고</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>FAIL 경보/조치</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2282,7 +2955,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2553,6 +3226,132 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_SETUP_REQUIRED</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MFA 설정 필요</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>OPS/ADMIN 계정에 MFA 미설정</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>MFA 등록 진행</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>계정 보안정책 확인</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>관리자 MFA 필수</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_INVALID_CODE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MFA 코드 불일치</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>TOTP 또는 복구코드 오류</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>코드 재확인</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>시간 동기화 확인</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>MFA 검증</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_LOCKED</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MFA 입력 잠금</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>반복 실패 누적</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Retry-After 후 재시도</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>실패 패턴 점검</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>잠금 해제까지</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>MFA brute-force 방어</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2564,7 +3363,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2715,6 +3514,114 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Node 22 표준 환경 확인</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>로컬/CI 재현성 확보</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>.nvmrc 기준 버전 확인</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>미완료</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>S2,S3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>권한/접근수준 구분 확인</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ROLE 혼동으로 인한 오판 방지</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>권한=ROLE, 비고=access_level 확인</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>미완료</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>S3,S4</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Runbook 최신본 확인</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>장애 대응 속도/정확도 확보</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>scheduler/audit/spec-notion runbook 숙지</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>미완료</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Notion 동기화 증적 확인</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>스펙-문서 분기 방지</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>spec_sync_report와 상태파일 점검</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>미완료</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>S4,S6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2726,7 +3633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2851,6 +3758,72 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>왜 관리자 로그인에서 인증을 두 번 하나요?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MFA 보안정책 때문입니다.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>OPS/ADMIN 계정은 탈취 위험이 높아 비밀번호 외 2차 인증을 필수로 적용합니다.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>권한 변경이 바로 적용되지 않는 이유는?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2인 승인 정책 때문입니다.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>RBAC 변경은 요청 생성 후 서로 다른 승인자 2명이 승인해야 실제 반영됩니다.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>S2,S3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Audit Chain Verify는 언제 쓰나요?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>감사로그 무결성 점검 시 사용합니다.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>정기 점검이나 이상 징후 발생 시 체인 검증을 실행하고 실패 시 runbook 절차로 대응합니다.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2862,7 +3835,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3039,6 +4012,102 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MFA 코드가 계속 틀렸다고 나옴</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>코드 불일치/시간 오차</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_INVALID_CODE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>기기 시간 자동동기화 후 재시도</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_INVALID_CODE</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MFA가 잠겨 로그인 불가</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>반복 실패로 잠금</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Retry-After 확인</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>잠금 해제 후 재시도/운영자 확인</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>AUTH_MFA_LOCKED</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>감사 무결성 점검 FAIL</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>chain hash 불연속</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>chain-verify 결과 확인</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>runbook_audit_chain 절차 실행</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: apply phase2.1.1 release hygiene hardening and refresh README
</commit_message>
<xml_diff>
--- a/menual/에이아이챗봇_통합_사용자_참조시트_20260221.xlsx
+++ b/menual/에이아이챗봇_통합_사용자_참조시트_20260221.xlsx
@@ -497,7 +497,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>S1(20260221 하드닝), S2(202603XX 종합보고서), S3(Go-Live Gap Closure), S4(spec_sync_report), S5(golive 증적)</t>
+          <t>S1(20260221 hardening), S2(202603XX full report), S3(Go-Live Gap Closure), S4(spec_sync_report), S5(phase2_1 evidence)</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:17:08Z</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:17:08Z</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:17:08Z</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:17:08Z</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>docs/review/mvp_verification_pack/artifacts/golive_spec_consistency_after.txt</t>
+          <t>docs/review/mvp_verification_pack/artifacts/phase2_1_pr2_spec_consistency_202603XX.txt</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:28:40Z</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -780,7 +780,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:28:40Z</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:28:40Z</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -829,27 +829,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Notion 동기화 완료 상태</t>
+          <t>Notion auto-sync blocked state (manual patch operation)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>docs/review/mvp_verification_pack/artifacts/golive_notion_sync_status.txt</t>
+          <t>docs/review/mvp_verification_pack/artifacts/phase2_1_pr2_notion_sync_status_202603XX.txt</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Status: DONE</t>
+          <t>status=BLOCKED_AUTOMATION</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:28:40Z</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>WARN</t>
         </is>
       </c>
     </row>
@@ -861,12 +861,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Go-Live UTF-8 검증 통과</t>
+          <t>Phase2.1 UTF-8 validation passed</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>docs/review/mvp_verification_pack/artifacts/golive_utf8_check.txt</t>
+          <t>docs/review/mvp_verification_pack/artifacts/phase2_1_utf8_check_202603XX.txt</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:28:40Z</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -908,7 +908,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2026-02-21T12:19:00Z</t>
+          <t>2026-02-21T14:28:40Z</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -928,7 +928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1026,6 +1026,50 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>S1,S2,S3,S4,S5,S6,S7</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>v2026.02.21-phase2.1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-02-21 23:17:08 +0900</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Phase2.1 PR1~PR3 ??(Notion fail-closed, async export-jobs, scheduler self-healing, ??/?? ???)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>S1,S2,S3,S4,S5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>v2026.02.21-phase2.1-r2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2026-02-21 23:28:40 +09:00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>menual consistency refresh (Notion status wording, phase2_1 evidence paths, risk wording normalization)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>S1,S2,S3,S4,S5,S6,S7</t>
         </is>

</xml_diff>